<commit_message>
Added clear button function that when clicked clears all entries
</commit_message>
<xml_diff>
--- a/Student_data.xlsx
+++ b/Student_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\PycharmProjects\untitled\Data Entry Form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FCE776-1CD8-462B-8A8C-BDFAC21E9C29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A2CCCB-3EA0-4229-A5D9-9642D6D23C64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="2085" windowWidth="16350" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Full Name</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>DOB</t>
+  </si>
+  <si>
+    <t>Faculty</t>
   </si>
 </sst>
 </file>
@@ -377,15 +380,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,6 +415,9 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made changes to the Insert button. after being clicked, it goes to new record
</commit_message>
<xml_diff>
--- a/Student_data.xlsx
+++ b/Student_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\PycharmProjects\untitled\Data Entry Form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A2CCCB-3EA0-4229-A5D9-9642D6D23C64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10CAB7C-B295-41E4-8A92-89EDCE281AA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="2085" windowWidth="16350" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed Bugs and finished styling the window
</commit_message>
<xml_diff>
--- a/Student_data.xlsx
+++ b/Student_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\PycharmProjects\untitled\Data Entry Form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10CAB7C-B295-41E4-8A92-89EDCE281AA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A2F3B1-244F-4709-A6A0-CD7F522791AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="2085" windowWidth="16350" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>